<commit_message>
completed all functioning tests: Note, all work was done pair programming excluding work done on 3-13 (Tyler Zudan's most recent commit). This work was done individually due to the large snowfall.
</commit_message>
<xml_diff>
--- a/ClueRooms_AdjTest.xlsx
+++ b/ClueRooms_AdjTest.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\eclipse-workspace\ClueGame\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC590EB-8C5D-4061-AE93-025CE5F12799}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="ClueRooms" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="32">
   <si>
     <t>C</t>
   </si>
@@ -102,28 +96,31 @@
     <t>JL</t>
   </si>
   <si>
-    <t>Light Purple: Locations with all walkway adjacencies</t>
-  </si>
-  <si>
-    <t>Orange: Locations within room with no adjs</t>
-  </si>
-  <si>
-    <t>Light Green: Locations at edge of board</t>
-  </si>
-  <si>
-    <t>Green: Locations beside doorway</t>
-  </si>
-  <si>
-    <t>White: Door</t>
-  </si>
-  <si>
-    <t>Light Yellow: More walkways to test</t>
+    <t>Orange: Test inside Room Adjacencies</t>
+  </si>
+  <si>
+    <t>Green: Room Exits Adjacencies</t>
+  </si>
+  <si>
+    <t>Purple: Adjacent to Doorways Adjacencies</t>
+  </si>
+  <si>
+    <t>Light Yellow: General Walkway Adjacencies</t>
+  </si>
+  <si>
+    <t>White: Walkway Targeting</t>
+  </si>
+  <si>
+    <t>Dark Gray: Room entrance Targeting</t>
+  </si>
+  <si>
+    <t>Light Blue: Room exit Targeting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,19 +163,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,7 +187,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -232,6 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,27 +508,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="5.7265625" customWidth="1"/>
+    <col min="1" max="26" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -542,7 +546,7 @@
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -600,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +620,7 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -677,7 +681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +697,7 @@
       <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -754,7 +758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +774,7 @@
       <c r="E4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -831,7 +835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -918,7 +922,7 @@
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -942,7 +946,7 @@
       <c r="K6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="M6" s="4" t="s">
@@ -985,7 +989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1013,10 +1017,10 @@
       <c r="I7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="J7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -1062,7 +1066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1117,7 +1121,7 @@
       <c r="R8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="S8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="T8" s="1" t="s">
@@ -1139,7 +1143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1216,8 +1220,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1265,10 +1269,10 @@
       <c r="P10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R10" s="8" t="s">
+      <c r="Q10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="S10" s="1" t="s">
@@ -1293,7 +1297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1370,14 +1374,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1386,7 +1390,7 @@
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -1422,10 +1426,10 @@
       <c r="Q12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R12" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="S12" s="10" t="s">
+      <c r="R12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="T12" s="1" t="s">
@@ -1447,7 +1451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1524,8 +1528,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1576,10 +1580,10 @@
       <c r="Q14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S14" s="3" t="s">
+      <c r="R14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" s="8" t="s">
         <v>1</v>
       </c>
       <c r="T14" s="3" t="s">
@@ -1601,7 +1605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -1638,7 +1642,7 @@
       <c r="L15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="8" t="s">
         <v>1</v>
       </c>
       <c r="N15" s="3" t="s">
@@ -1665,7 +1669,7 @@
       <c r="U15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V15" s="4" t="s">
+      <c r="V15" s="10" t="s">
         <v>22</v>
       </c>
       <c r="W15" s="1" t="s">
@@ -1678,14 +1682,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1755,7 +1759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1774,7 +1778,7 @@
       <c r="F17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -1783,7 +1787,7 @@
       <c r="I17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -1832,7 +1836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1909,7 +1913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1961,7 +1965,7 @@
       <c r="Q19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R19" s="3" t="s">
+      <c r="R19" s="12" t="s">
         <v>1</v>
       </c>
       <c r="S19" s="4" t="s">
@@ -1986,7 +1990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -2002,10 +2006,10 @@
       <c r="E20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -2020,7 +2024,7 @@
       <c r="K20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="12" t="s">
         <v>1</v>
       </c>
       <c r="M20" s="4" t="s">
@@ -2063,7 +2067,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -2140,7 +2144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -2189,7 +2193,7 @@
       <c r="P22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q22" s="3" t="s">
+      <c r="Q22" s="8" t="s">
         <v>1</v>
       </c>
       <c r="R22" s="3" t="s">
@@ -2217,7 +2221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2294,7 +2298,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2368,34 +2372,39 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:25" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>